<commit_message>
trans/AVLRaPTC updating to EU specific data
</commit_message>
<xml_diff>
--- a/InputData/trans/AVLRaPTC/Annual Vehicle Licensing Registration and Property Tax Costs.xlsx
+++ b/InputData/trans/AVLRaPTC/Annual Vehicle Licensing Registration and Property Tax Costs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\trans\AVLRaPTC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claire Trevisan\Dropbox (Energy Innovation)\Documents\GitHub\eps-eu\InputData\trans\AVLRaPTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D32A06-ED03-485E-BDB4-2BF12EEC6254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86A0B8F-D777-4067-860F-3FD0B80394D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33735" yWindow="675" windowWidth="21600" windowHeight="22305" xr2:uid="{AF599D04-C13D-45D7-BEF0-770B4B16FC27}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AF599D04-C13D-45D7-BEF0-770B4B16FC27}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
   <si>
     <t>Sources:</t>
   </si>
@@ -43,63 +43,18 @@
     <t>Data</t>
   </si>
   <si>
-    <t>American Automobile Association</t>
-  </si>
-  <si>
     <t>https://www.aaa.com/autorepair/articles/average-annual-cost-of-new-vehicle-ownership</t>
   </si>
   <si>
-    <t>Average Annual Cost of New Car Ownership Increases 5% to $9,282</t>
-  </si>
-  <si>
-    <t>Explanation and Examples of U.S. State Vehicle Property Taxes</t>
-  </si>
-  <si>
-    <t>Hendrickson, V. L.</t>
-  </si>
-  <si>
-    <t>Which U.S. States Charge Property Taxes for Cars?</t>
-  </si>
-  <si>
-    <t>https://www.mansionglobal.com/articles/which-u-s-states-charge-property-taxes-for-cars-220298</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
     <t>The AAA document cited above lists the average U.S.-wide annual cost of licensing, registration, and taxes as:</t>
   </si>
   <si>
-    <t>2019 USD/year</t>
-  </si>
-  <si>
-    <t>This might seem high if one is familiar with annual license plate and car registration fees in some states,</t>
-  </si>
-  <si>
-    <t>but it is likely reasonable when property tax is factored in.  Property tax on vehicles varies greatly by state,</t>
-  </si>
-  <si>
-    <t>with 23 states not charging it at all, versus the highest state charging an average of $1,011/year</t>
-  </si>
-  <si>
-    <t>(according to Hendrickson, cited above).  The AAA number appears to be a reasonable average accounting for</t>
-  </si>
-  <si>
-    <t>high property taxes in some states and vehicle registration and license fees in essentially all states.</t>
-  </si>
-  <si>
-    <t>The AAA number does not include sales tax on the car's initial purchase, which also varies by state, but</t>
-  </si>
-  <si>
-    <t>generally is much higher than $753 (since the U.S. average sales tax is over 7%).</t>
-  </si>
-  <si>
     <t>Currency Conversion</t>
   </si>
   <si>
-    <t>2019 to 2021 USD</t>
-  </si>
-  <si>
     <t>2012 USD/year</t>
   </si>
   <si>
@@ -140,16 +95,152 @@
   </si>
   <si>
     <t>AVLRaPTC Annual Vehicle Licensing Registration and Property Tax Costs</t>
+  </si>
+  <si>
+    <t>European Automobile Manufacturers’ Association (ACEA)</t>
+  </si>
+  <si>
+    <t>Interactive map – Tax revenue per motor vehicle in major EU markets</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Average annual tax revenue per motor vehicle, by country</t>
+  </si>
+  <si>
+    <t>Average Total</t>
+  </si>
+  <si>
+    <t>Fuel and Lubricant Taxes</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>https://www.acea.auto/publication/acea-tax-guide-2022/</t>
+  </si>
+  <si>
+    <t>ACEA Tax Guide 2022</t>
+  </si>
+  <si>
+    <t>Tax revenue from fuel and lubricant taxes</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>Percent of Total contributed by Fuels/Lubricants</t>
+  </si>
+  <si>
+    <t>2022 Euro/year</t>
+  </si>
+  <si>
+    <t>2022 Euro to USD</t>
+  </si>
+  <si>
+    <t>2022 to 2012 USD</t>
+  </si>
+  <si>
+    <t>This number reflects an average annual cost across the countries with available data in the EU.</t>
+  </si>
+  <si>
+    <t>Average Percentage of Total Fiscal Income from Vehicles from Fuel and Lubricant Taxes</t>
+  </si>
+  <si>
+    <t>The average amount of fiscal income from fuel and lubricant taxes is excluded from this value because it is captured elsewhere in the EPS model.</t>
+  </si>
+  <si>
+    <t>Licensing, registration, and tax structures and amounts range by country, but this average should capture the variation and reflect the total revenue.</t>
+  </si>
+  <si>
+    <t>2022 USD/year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="[$€-2]\ #,##0.00_);[Red]\([$€-2]\ #,##0.00\)"/>
+    <numFmt numFmtId="168" formatCode="[$€-2]\ #,##0;[Red]\-[$€-2]\ #,##0"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="174" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +263,30 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF002D41"/>
+      <name val="Roboto Condensed"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF002D41"/>
+      <name val="Roboto Condensed"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF002D41"/>
+      <name val="Roboto Condensed"/>
     </font>
   </fonts>
   <fills count="5">
@@ -209,11 +324,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -221,7 +338,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="6" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -230,10 +346,34 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -246,6 +386,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>457514</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>82776</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23DBBED2-3097-52A8-3C47-83694533A671}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12182475" y="444500"/>
+          <a:ext cx="6105839" cy="4391251"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>85805</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>28983</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>73216</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DF82CB1-5D6E-D1F5-BBDD-E54DAEFF255A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11792030" y="5511800"/>
+          <a:ext cx="6645603" cy="3114866"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -545,21 +778,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC3CD7F-A224-4C3A-9A5E-D38F07B136AE}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="61.42578125" customWidth="1"/>
+    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.453125" customWidth="1"/>
+    <col min="9" max="9" width="17.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,161 +804,454 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.35">
+      <c r="B5" s="3">
+        <v>2022</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="10">
+        <v>2892</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="H7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="10">
+        <v>2723</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="H8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="10">
+        <v>2438</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="B9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="10">
+        <v>2409</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="10">
+        <v>2217</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="24" x14ac:dyDescent="0.35">
+      <c r="B11" s="3">
+        <v>2022</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="10">
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="10">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="10">
+        <v>1727</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="H14" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="10">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="10">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="23" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="H16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="10">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="23" x14ac:dyDescent="0.35">
+      <c r="A17" s="18">
+        <f>A18*A40</f>
+        <v>1091.7837795046976</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="I17" s="10">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="23" x14ac:dyDescent="0.35">
+      <c r="A18" s="15">
+        <f>I19*(1-K37)</f>
+        <v>1036.0445810445033</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="10">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="24" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="13">
+        <f>AVERAGE(I6:I18)</f>
+        <v>1938.4615384615386</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="I23" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="J23" t="s">
+        <v>38</v>
+      </c>
+      <c r="K23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H24" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J24">
+        <v>13.4</v>
+      </c>
+      <c r="K24" s="14">
+        <f>I24/J24</f>
+        <v>0.34328358208955223</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I25">
+        <v>7.3</v>
+      </c>
+      <c r="J25">
+        <v>19.600000000000001</v>
+      </c>
+      <c r="K25" s="14">
+        <f t="shared" ref="K25:K36" si="0">I25/J25</f>
+        <v>0.3724489795918367</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I26">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="J26">
+        <v>89.7</v>
+      </c>
+      <c r="K26" s="14">
+        <f t="shared" si="0"/>
+        <v>0.4202898550724638</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H27" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27">
+        <v>17.3</v>
+      </c>
+      <c r="J27">
+        <v>48.8</v>
+      </c>
+      <c r="K27" s="14">
+        <f t="shared" si="0"/>
+        <v>0.35450819672131151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="H28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28">
+        <v>20.5</v>
+      </c>
+      <c r="J28">
+        <v>34.1</v>
+      </c>
+      <c r="K28" s="14">
+        <f t="shared" si="0"/>
+        <v>0.60117302052785926</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" t="s">
+        <v>47</v>
+      </c>
+      <c r="I29">
+        <v>3.9</v>
+      </c>
+      <c r="J29">
+        <v>8.6</v>
+      </c>
+      <c r="K29" s="14">
+        <f t="shared" si="0"/>
+        <v>0.45348837209302328</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="H30" t="s">
+        <v>48</v>
+      </c>
+      <c r="I30">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="J30">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="K30" s="14">
+        <f t="shared" si="0"/>
+        <v>0.47956403269754766</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" s="8">
+        <v>2</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31" t="s">
+        <v>49</v>
+      </c>
+      <c r="I31">
+        <v>5.5</v>
+      </c>
+      <c r="J31">
+        <v>8.1</v>
+      </c>
+      <c r="K31" s="14">
+        <f t="shared" si="0"/>
+        <v>0.67901234567901236</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" s="8">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32" t="s">
+        <v>50</v>
+      </c>
+      <c r="I32">
+        <v>3.5</v>
+      </c>
+      <c r="J32">
+        <v>6.2</v>
+      </c>
+      <c r="K32" s="14">
+        <f t="shared" si="0"/>
+        <v>0.56451612903225801</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H33" t="s">
+        <v>51</v>
+      </c>
+      <c r="I33">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="J33">
+        <v>76.3</v>
+      </c>
+      <c r="K33" s="14">
+        <f t="shared" si="0"/>
+        <v>0.48885976408912185</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>753</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="B30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
-        <v>2</v>
-      </c>
-      <c r="B31" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>0.89800000000000002</v>
+      <c r="H34" t="s">
+        <v>52</v>
+      </c>
+      <c r="I34">
+        <v>10.4</v>
+      </c>
+      <c r="J34">
+        <v>21.5</v>
+      </c>
+      <c r="K34" s="14">
+        <f t="shared" si="0"/>
+        <v>0.48372093023255813</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H35" t="s">
+        <v>53</v>
+      </c>
+      <c r="I35">
+        <v>2.8</v>
+      </c>
+      <c r="J35">
+        <v>8.5</v>
+      </c>
+      <c r="K35" s="14">
+        <f t="shared" si="0"/>
+        <v>0.32941176470588235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A36" s="16">
+        <v>0.78553197418898923</v>
       </c>
       <c r="B36" t="s">
-        <v>20</v>
+        <v>58</v>
+      </c>
+      <c r="H36" t="s">
+        <v>54</v>
+      </c>
+      <c r="I36">
+        <v>43.3</v>
+      </c>
+      <c r="J36">
+        <v>89.9</v>
+      </c>
+      <c r="K36" s="14">
+        <f t="shared" si="0"/>
+        <v>0.48164627363737478</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I37" s="1"/>
+      <c r="J37" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K37" s="20">
+        <f>AVERAGE(K24:K36)</f>
+        <v>0.46553255739767702</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A40" s="17">
+        <v>1.0538000000000001</v>
+      </c>
+      <c r="B40" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{40391687-33E8-4157-BFF1-4B9C3152973E}"/>
-    <hyperlink ref="B13" r:id="rId2" xr:uid="{ACA01131-F87A-4018-B151-91F58C3F8660}"/>
+    <hyperlink ref="B13" r:id="rId2" xr:uid="{10D2D38D-CA79-4D0E-9B5C-2BF96667770D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -732,54 +1262,56 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="3" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="3" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="8">
+        <v>9</v>
+      </c>
+      <c r="B2" s="7">
         <f>About!A17*About!$A$36</f>
-        <v>676.19399999999996</v>
-      </c>
-      <c r="C2" s="8">
+        <v>857.63106770184118</v>
+      </c>
+      <c r="C2" s="7">
         <f>$B$2*About!$A$32</f>
-        <v>676.19399999999996</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>857.63106770184118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="8">
+        <v>10</v>
+      </c>
+      <c r="B3" s="7">
         <f>$B$2*About!$A$31</f>
-        <v>1352.3879999999999</v>
-      </c>
-      <c r="C3" s="8">
+        <v>1715.2621354036824</v>
+      </c>
+      <c r="C3" s="7">
         <f>$B$2*About!$A$31</f>
-        <v>1352.3879999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1715.2621354036824</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -788,9 +1320,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -799,9 +1331,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -810,13 +1342,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="8">
+        <v>14</v>
+      </c>
+      <c r="B7" s="7">
         <f>$B$2*About!$A$30</f>
-        <v>338.09699999999998</v>
+        <v>428.81553385092059</v>
       </c>
       <c r="C7">
         <v>0</v>

</xml_diff>